<commit_message>
Update 1.5.6: Bug fixes
</commit_message>
<xml_diff>
--- a/pkg/excels/templates/output.xlsx
+++ b/pkg/excels/templates/output.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mamad\OneDrive\Desktop\ТГЭМ\backend-v2\pkg\excels\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16F91DB-157F-4CE4-8153-CE4994E2B051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB75629-C79C-4DD7-B674-B5D4E0A1A5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
-  <si>
-    <t xml:space="preserve">Адресс объекта: </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t xml:space="preserve"> Гос. номер: </t>
   </si>
@@ -101,9 +98,6 @@
     <t>ОАО  "ТГЭМ"</t>
   </si>
   <si>
-    <t xml:space="preserve">Объект: </t>
-  </si>
-  <si>
     <t>Отпуск разр.:</t>
   </si>
   <si>
@@ -111,32 +105,6 @@
   </si>
   <si>
     <t>_________</t>
-  </si>
-  <si>
-    <r>
-      <t>Катег. объекта:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
   </si>
   <si>
     <t>Мухаммадиев М.</t>
@@ -264,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -327,9 +295,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -698,7 +663,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="163" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,61 +678,55 @@
   <sheetData>
     <row r="1" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>14</v>
       </c>
       <c r="E1" s="18"/>
       <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="A2" s="4"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
-      <c r="D2" s="19" t="s">
-        <v>0</v>
-      </c>
+      <c r="D2" s="19"/>
       <c r="E2" s="19"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>16</v>
-      </c>
+      <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="22"/>
     </row>
     <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="C4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="D4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="F4" s="11" t="s">
         <v>6</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -780,14 +739,14 @@
     </row>
     <row r="6" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
         <v>17</v>
-      </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -796,21 +755,21 @@
     </row>
     <row r="8" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="1"/>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="21"/>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -821,11 +780,11 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="21"/>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -834,14 +793,14 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="21"/>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 1.6.5.6: Bug fix
</commit_message>
<xml_diff>
--- a/pkg/excels/templates/output.xlsx
+++ b/pkg/excels/templates/output.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mamad\OneDrive\Desktop\ТГЭМ\backend-v2\pkg\excels\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\TGEM\tgem-backend\pkg\excels\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB75629-C79C-4DD7-B674-B5D4E0A1A5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Отпуск" sheetId="2" r:id="rId1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t xml:space="preserve"> Гос. номер: </t>
   </si>
@@ -106,14 +105,11 @@
   <si>
     <t>_________</t>
   </si>
-  <si>
-    <t>Мухаммадиев М.</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -298,7 +294,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -659,11 +655,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928E14FB-753C-4C9C-8CE9-5FF3781C0E0E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="163" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,14 +733,12 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="21"/>
-      <c r="C6" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="C6" s="4"/>
       <c r="E6" t="s">
         <v>17</v>
       </c>
@@ -753,7 +747,7 @@
       <c r="A7" s="1"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>11</v>
       </c>

</xml_diff>